<commit_message>
test tanbahan baru di file xlsx
</commit_message>
<xml_diff>
--- a/Shopee 2207/Shopee 220719.xlsx
+++ b/Shopee 2207/Shopee 220719.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="288">
   <si>
     <t>No. Pesanan</t>
   </si>
@@ -876,6 +876,9 @@
   </si>
   <si>
     <t>KOTA MALANG</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -940,7 +943,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -983,11 +986,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1009,6 +1021,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3838,10 +3853,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.7109375" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3913,7 +3928,16 @@
         <v>279</v>
       </c>
     </row>
+    <row r="9" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B9" s="8"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:B9"/>
+  </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="142" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>